<commit_message>
update test results for new model 2 t/l ratio calculation
</commit_message>
<xml_diff>
--- a/test/gait/data/manual_gait_results_apcwt.xlsx
+++ b/test/gait/data/manual_gait_results_apcwt.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11008"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11028"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lukasadamowicz/Documents/Packages/scikit-digital-health/test/gaitv3/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lukasadamowicz/Documents/Packages/scikit-digital-health/test/gait/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85189C5E-1372-2C43-97EC-D6932C5AF061}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25532FA6-7C37-0444-B171-A23E190CEA82}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="31720" windowHeight="24660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -633,12 +633,11 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1023,8 +1022,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AG82"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="N24" workbookViewId="0">
-      <selection activeCell="AG82" sqref="AG82"/>
+    <sheetView tabSelected="1" topLeftCell="J28" workbookViewId="0">
+      <selection activeCell="AB53" sqref="AB53:AB81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1221,24 +1220,24 @@
         <v>0.39999999999999997</v>
       </c>
       <c r="AB2">
-        <f>1.12 * AA2 * AA2 + 0.547 * AA2 + 0.066</f>
-        <v>0.46400000000000002</v>
+        <f>1.1 * AA2</f>
+        <v>0.44</v>
       </c>
       <c r="AC2">
         <f>AB2*P2</f>
-        <v>0.46232960000000001</v>
+        <v>0.43841599999999997</v>
       </c>
       <c r="AD2">
         <f>2 * SQRT(2 * P2 * N2 - N2 * N2) + 2 * SQRT(2 * AC2 * O2 - O2 * O2)</f>
-        <v>0.86023938160987679</v>
+        <v>0.85222144820780854</v>
       </c>
       <c r="AE2">
         <f>AD2+AD3</f>
-        <v>1.6002654548416915</v>
+        <v>1.5870037139405293</v>
       </c>
       <c r="AF2">
         <f>AE2/R2</f>
-        <v>1.3561571651200777</v>
+        <v>1.3449184016445164</v>
       </c>
       <c r="AG2">
         <f>60/Q2</f>
@@ -1336,24 +1335,24 @@
         <v>0.39999999999999997</v>
       </c>
       <c r="AB3">
-        <f t="shared" ref="AB3:AB66" si="11">1.12 * AA3 * AA3 + 0.547 * AA3 + 0.066</f>
-        <v>0.46400000000000002</v>
+        <f t="shared" ref="AB3:AB50" si="11">1.1 * AA3</f>
+        <v>0.44</v>
       </c>
       <c r="AC3">
         <f t="shared" ref="AC3:AC66" si="12">AB3*P3</f>
-        <v>0.46232960000000001</v>
+        <v>0.43841599999999997</v>
       </c>
       <c r="AD3">
         <f t="shared" ref="AD3:AD66" si="13">2 * SQRT(2 * P3 * N3 - N3 * N3) + 2 * SQRT(2 * AC3 * O3 - O3 * O3)</f>
-        <v>0.74002607323181469</v>
+        <v>0.73478226573272076</v>
       </c>
       <c r="AE3">
         <f t="shared" ref="AE3:AE66" si="14">AD3+AD4</f>
-        <v>1.482942965539817</v>
+        <v>1.4717247312446835</v>
       </c>
       <c r="AF3">
         <f t="shared" ref="AF3:AF66" si="15">AE3/R3</f>
-        <v>1.3240562192319794</v>
+        <v>1.3140399386113244</v>
       </c>
       <c r="AG3">
         <f t="shared" ref="AG3:AG66" si="16">60/Q3</f>
@@ -1452,23 +1451,23 @@
       </c>
       <c r="AB4">
         <f t="shared" si="11"/>
-        <v>0.46400000000000002</v>
+        <v>0.44</v>
       </c>
       <c r="AC4">
         <f t="shared" si="12"/>
-        <v>0.46232960000000001</v>
+        <v>0.43841599999999997</v>
       </c>
       <c r="AD4">
         <f t="shared" si="13"/>
-        <v>0.74291689230800217</v>
+        <v>0.73694246551196285</v>
       </c>
       <c r="AE4">
         <f t="shared" si="14"/>
-        <v>1.4554794239072835</v>
+        <v>1.4445478743900666</v>
       </c>
       <c r="AF4">
         <f t="shared" si="15"/>
-        <v>1.3231631126429848</v>
+        <v>1.3132253403546059</v>
       </c>
       <c r="AG4">
         <f t="shared" si="16"/>
@@ -1567,23 +1566,23 @@
       </c>
       <c r="AB5">
         <f t="shared" si="11"/>
-        <v>0.46400000000000002</v>
+        <v>0.44</v>
       </c>
       <c r="AC5">
         <f t="shared" si="12"/>
-        <v>0.46232960000000001</v>
+        <v>0.43841599999999997</v>
       </c>
       <c r="AD5">
         <f t="shared" si="13"/>
-        <v>0.71256253159928118</v>
+        <v>0.70760540887810386</v>
       </c>
       <c r="AE5">
         <f t="shared" si="14"/>
-        <v>1.4789602646429305</v>
+        <v>1.4676884000151618</v>
       </c>
       <c r="AF5">
         <f t="shared" si="15"/>
-        <v>1.344509331493573</v>
+        <v>1.3342621818319651</v>
       </c>
       <c r="AG5">
         <f t="shared" si="16"/>
@@ -1682,23 +1681,23 @@
       </c>
       <c r="AB6">
         <f t="shared" si="11"/>
-        <v>0.46400000000000002</v>
+        <v>0.44</v>
       </c>
       <c r="AC6">
         <f t="shared" si="12"/>
-        <v>0.46232960000000001</v>
+        <v>0.43841599999999997</v>
       </c>
       <c r="AD6">
         <f t="shared" si="13"/>
-        <v>0.76639773304364922</v>
+        <v>0.76008299113705791</v>
       </c>
       <c r="AE6">
         <f t="shared" si="14"/>
-        <v>1.5922430810469161</v>
+        <v>1.5798631122162623</v>
       </c>
       <c r="AF6">
         <f t="shared" si="15"/>
-        <v>1.3967044570586984</v>
+        <v>1.3858448352774231</v>
       </c>
       <c r="AG6">
         <f t="shared" si="16"/>
@@ -1797,23 +1796,23 @@
       </c>
       <c r="AB7">
         <f t="shared" si="11"/>
-        <v>0.46400000000000002</v>
+        <v>0.44</v>
       </c>
       <c r="AC7">
         <f t="shared" si="12"/>
-        <v>0.46232960000000001</v>
+        <v>0.43841599999999997</v>
       </c>
       <c r="AD7">
         <f t="shared" si="13"/>
-        <v>0.82584534800326692</v>
+        <v>0.81978012107920439</v>
       </c>
       <c r="AE7">
         <f t="shared" si="14"/>
-        <v>1.5757155269038627</v>
+        <v>1.5642131293289032</v>
       </c>
       <c r="AF7">
         <f t="shared" si="15"/>
-        <v>1.4068888633070202</v>
+        <v>1.3966188654722349</v>
       </c>
       <c r="AG7">
         <f t="shared" si="16"/>
@@ -1912,23 +1911,23 @@
       </c>
       <c r="AB8">
         <f t="shared" si="11"/>
-        <v>0.46400000000000002</v>
+        <v>0.44</v>
       </c>
       <c r="AC8">
         <f t="shared" si="12"/>
-        <v>0.46232960000000001</v>
+        <v>0.43841599999999997</v>
       </c>
       <c r="AD8">
         <f t="shared" si="13"/>
-        <v>0.74987017890059582</v>
+        <v>0.74443300824969871</v>
       </c>
       <c r="AE8">
         <f t="shared" si="14"/>
-        <v>1.503938813528545</v>
+        <v>1.4927482867180277</v>
       </c>
       <c r="AF8">
         <f t="shared" si="15"/>
-        <v>1.4188102014420234</v>
+        <v>1.4082531006773846</v>
       </c>
       <c r="AG8">
         <f t="shared" si="16"/>
@@ -2027,23 +2026,23 @@
       </c>
       <c r="AB9">
         <f t="shared" si="11"/>
-        <v>0.46400000000000002</v>
+        <v>0.44</v>
       </c>
       <c r="AC9">
         <f t="shared" si="12"/>
-        <v>0.46232960000000001</v>
+        <v>0.43841599999999997</v>
       </c>
       <c r="AD9">
         <f t="shared" si="13"/>
-        <v>0.75406863462794915</v>
+        <v>0.74831527846832901</v>
       </c>
       <c r="AE9">
         <f t="shared" si="14"/>
-        <v>1.5757814400795942</v>
+        <v>1.5633469722282132</v>
       </c>
       <c r="AF9">
         <f t="shared" si="15"/>
-        <v>1.4865862642260321</v>
+        <v>1.4748556341775596</v>
       </c>
       <c r="AG9">
         <f t="shared" si="16"/>
@@ -2142,23 +2141,23 @@
       </c>
       <c r="AB10">
         <f t="shared" si="11"/>
-        <v>0.46400000000000002</v>
+        <v>0.44</v>
       </c>
       <c r="AC10">
         <f t="shared" si="12"/>
-        <v>0.46232960000000001</v>
+        <v>0.43841599999999997</v>
       </c>
       <c r="AD10">
         <f t="shared" si="13"/>
-        <v>0.82171280545164516</v>
+        <v>0.81503169375988416</v>
       </c>
       <c r="AE10">
         <f t="shared" si="14"/>
-        <v>1.6204206050106773</v>
+        <v>1.607842338031245</v>
       </c>
       <c r="AF10">
         <f t="shared" si="15"/>
-        <v>1.5003894490839604</v>
+        <v>1.4887429055844861</v>
       </c>
       <c r="AG10">
         <f t="shared" si="16"/>
@@ -2257,23 +2256,23 @@
       </c>
       <c r="AB11">
         <f t="shared" si="11"/>
-        <v>0.46400000000000002</v>
+        <v>0.44</v>
       </c>
       <c r="AC11">
         <f t="shared" si="12"/>
-        <v>0.46232960000000001</v>
+        <v>0.43841599999999997</v>
       </c>
       <c r="AD11">
         <f t="shared" si="13"/>
-        <v>0.79870779955903226</v>
+        <v>0.79281064427136072</v>
       </c>
       <c r="AE11">
         <f t="shared" si="14"/>
-        <v>1.6206560330297686</v>
+        <v>1.6082041788579979</v>
       </c>
       <c r="AF11">
         <f t="shared" si="15"/>
-        <v>1.5006074379905263</v>
+        <v>1.4890779433870349</v>
       </c>
       <c r="AG11">
         <f t="shared" si="16"/>
@@ -2372,23 +2371,23 @@
       </c>
       <c r="AB12">
         <f t="shared" si="11"/>
-        <v>0.46400000000000002</v>
+        <v>0.44</v>
       </c>
       <c r="AC12">
         <f t="shared" si="12"/>
-        <v>0.46232960000000001</v>
+        <v>0.43841599999999997</v>
       </c>
       <c r="AD12">
         <f t="shared" si="13"/>
-        <v>0.82194823347073642</v>
+        <v>0.81539353458663733</v>
       </c>
       <c r="AE12">
         <f t="shared" si="14"/>
-        <v>1.6340139268671718</v>
+        <v>1.6205559325400385</v>
       </c>
       <c r="AF12">
         <f t="shared" si="15"/>
-        <v>1.5711672373722805</v>
+        <v>1.5582268582115755</v>
       </c>
       <c r="AG12">
         <f t="shared" si="16"/>
@@ -2487,23 +2486,23 @@
       </c>
       <c r="AB13">
         <f t="shared" si="11"/>
-        <v>0.46400000000000002</v>
+        <v>0.44</v>
       </c>
       <c r="AC13">
         <f t="shared" si="12"/>
-        <v>0.46232960000000001</v>
+        <v>0.43841599999999997</v>
       </c>
       <c r="AD13">
         <f t="shared" si="13"/>
-        <v>0.81206569339643542</v>
+        <v>0.80516239795340128</v>
       </c>
       <c r="AE13">
         <f t="shared" si="14"/>
-        <v>1.7395910841685518</v>
+        <v>1.7244855689503273</v>
       </c>
       <c r="AF13">
         <f t="shared" si="15"/>
-        <v>1.6107324853412515</v>
+        <v>1.5967458971762289</v>
       </c>
       <c r="AG13">
         <f t="shared" si="16"/>
@@ -2602,23 +2601,23 @@
       </c>
       <c r="AB14">
         <f t="shared" si="11"/>
-        <v>0.46400000000000002</v>
+        <v>0.44</v>
       </c>
       <c r="AC14">
         <f t="shared" si="12"/>
-        <v>0.46232960000000001</v>
+        <v>0.43841599999999997</v>
       </c>
       <c r="AD14">
         <f t="shared" si="13"/>
-        <v>0.92752539077211638</v>
+        <v>0.91932317099692618</v>
       </c>
       <c r="AE14">
         <f t="shared" si="14"/>
-        <v>1.7398720551008175</v>
+        <v>1.7248467673568815</v>
       </c>
       <c r="AF14">
         <f t="shared" si="15"/>
-        <v>1.610992643611868</v>
+        <v>1.5970803401452605</v>
       </c>
       <c r="AG14">
         <f t="shared" si="16"/>
@@ -2717,23 +2716,23 @@
       </c>
       <c r="AB15">
         <f t="shared" si="11"/>
-        <v>0.46400000000000002</v>
+        <v>0.44</v>
       </c>
       <c r="AC15">
         <f t="shared" si="12"/>
-        <v>0.46232960000000001</v>
+        <v>0.43841599999999997</v>
       </c>
       <c r="AD15">
         <f t="shared" si="13"/>
-        <v>0.81234666432870117</v>
+        <v>0.80552359635995541</v>
       </c>
       <c r="AE15">
         <f t="shared" si="14"/>
-        <v>1.7163114840596405</v>
+        <v>1.7017971353791099</v>
       </c>
       <c r="AF15">
         <f t="shared" si="15"/>
-        <v>1.5602831673269457</v>
+        <v>1.5470883048900999</v>
       </c>
       <c r="AG15">
         <f t="shared" si="16"/>
@@ -2832,23 +2831,23 @@
       </c>
       <c r="AB16">
         <f t="shared" si="11"/>
-        <v>0.46400000000000002</v>
+        <v>0.44</v>
       </c>
       <c r="AC16">
         <f t="shared" si="12"/>
-        <v>0.46232960000000001</v>
+        <v>0.43841599999999997</v>
       </c>
       <c r="AD16">
         <f t="shared" si="13"/>
-        <v>0.90396481973093934</v>
+        <v>0.89627353901915452</v>
       </c>
       <c r="AE16">
         <f t="shared" si="14"/>
-        <v>1.6058334577214035</v>
+        <v>1.5928120971217805</v>
       </c>
       <c r="AF16">
         <f t="shared" si="15"/>
-        <v>1.4337798729655387</v>
+        <v>1.4221536581444467</v>
       </c>
       <c r="AG16">
         <f t="shared" si="16"/>
@@ -2947,23 +2946,23 @@
       </c>
       <c r="AB17">
         <f t="shared" si="11"/>
-        <v>0.46400000000000002</v>
+        <v>0.44</v>
       </c>
       <c r="AC17">
         <f t="shared" si="12"/>
-        <v>0.46232960000000001</v>
+        <v>0.43841599999999997</v>
       </c>
       <c r="AD17">
         <f t="shared" si="13"/>
-        <v>0.70186863799046406</v>
+        <v>0.69653855810262599</v>
       </c>
       <c r="AE17">
         <f t="shared" si="14"/>
-        <v>1.6328848915003746</v>
+        <v>1.619195014171962</v>
       </c>
       <c r="AF17">
         <f t="shared" si="15"/>
-        <v>1.4323551679827848</v>
+        <v>1.4203465036596159</v>
       </c>
       <c r="AG17">
         <f t="shared" si="16"/>
@@ -3062,23 +3061,23 @@
       </c>
       <c r="AB18">
         <f t="shared" si="11"/>
-        <v>0.46400000000000002</v>
+        <v>0.44</v>
       </c>
       <c r="AC18">
         <f t="shared" si="12"/>
-        <v>0.46232960000000001</v>
+        <v>0.43841599999999997</v>
       </c>
       <c r="AD18">
         <f t="shared" si="13"/>
-        <v>0.93101625350991046</v>
+        <v>0.922656456069336</v>
       </c>
       <c r="AE18">
         <f t="shared" si="14"/>
-        <v>1.6282676560243692</v>
+        <v>1.6149824206554855</v>
       </c>
       <c r="AF18">
         <f t="shared" si="15"/>
-        <v>1.3346456196921059</v>
+        <v>1.3237560825044963</v>
       </c>
       <c r="AG18">
         <f t="shared" si="16"/>
@@ -3177,23 +3176,23 @@
       </c>
       <c r="AB19">
         <f t="shared" si="11"/>
-        <v>0.46400000000000002</v>
+        <v>0.44</v>
       </c>
       <c r="AC19">
         <f t="shared" si="12"/>
-        <v>0.46232960000000001</v>
+        <v>0.43841599999999997</v>
       </c>
       <c r="AD19">
         <f t="shared" si="13"/>
-        <v>0.69725140251445872</v>
+        <v>0.69232596458614948</v>
       </c>
       <c r="AE19">
         <f t="shared" si="14"/>
-        <v>1.3681771332639601</v>
+        <v>1.3588421142300073</v>
       </c>
       <c r="AF19">
         <f t="shared" si="15"/>
-        <v>1.2001553800561053</v>
+        <v>1.1919667668684275</v>
       </c>
       <c r="AG19">
         <f t="shared" si="16"/>
@@ -3292,23 +3291,23 @@
       </c>
       <c r="AB20">
         <f t="shared" si="11"/>
-        <v>0.46400000000000002</v>
+        <v>0.44</v>
       </c>
       <c r="AC20">
         <f t="shared" si="12"/>
-        <v>0.46232960000000001</v>
+        <v>0.43841599999999997</v>
       </c>
       <c r="AD20">
         <f t="shared" si="13"/>
-        <v>0.67092573074950146</v>
+        <v>0.66651614964385786</v>
       </c>
       <c r="AE20">
         <f t="shared" si="14"/>
-        <v>1.4484101547555315</v>
+        <v>1.4383575932403949</v>
       </c>
       <c r="AF20">
         <f t="shared" si="15"/>
-        <v>1.3167365043232104</v>
+        <v>1.3075978120367227</v>
       </c>
       <c r="AG20">
         <f t="shared" si="16"/>
@@ -3407,23 +3406,23 @@
       </c>
       <c r="AB21">
         <f t="shared" si="11"/>
-        <v>0.46400000000000002</v>
+        <v>0.44</v>
       </c>
       <c r="AC21">
         <f t="shared" si="12"/>
-        <v>0.46232960000000001</v>
+        <v>0.43841599999999997</v>
       </c>
       <c r="AD21">
         <f t="shared" si="13"/>
-        <v>0.77748442400603013</v>
+        <v>0.77184144359653706</v>
       </c>
       <c r="AE21">
         <f t="shared" si="14"/>
-        <v>1.4853504623847731</v>
+        <v>1.4746170679096033</v>
       </c>
       <c r="AF21">
         <f t="shared" si="15"/>
-        <v>1.3503186021679754</v>
+        <v>1.3405609708269119</v>
       </c>
       <c r="AG21">
         <f t="shared" si="16"/>
@@ -3522,23 +3521,23 @@
       </c>
       <c r="AB22">
         <f t="shared" si="11"/>
-        <v>0.46400000000000002</v>
+        <v>0.44</v>
       </c>
       <c r="AC22">
         <f t="shared" si="12"/>
-        <v>0.46232960000000001</v>
+        <v>0.43841599999999997</v>
       </c>
       <c r="AD22">
         <f t="shared" si="13"/>
-        <v>0.70786603837874307</v>
+        <v>0.70277562431306628</v>
       </c>
       <c r="AE22">
         <f t="shared" si="14"/>
-        <v>1.4439321617290042</v>
+        <v>1.4337029425805627</v>
       </c>
       <c r="AF22">
         <f t="shared" si="15"/>
-        <v>1.3369742238231519</v>
+        <v>1.327502724611632</v>
       </c>
       <c r="AG22">
         <f t="shared" si="16"/>
@@ -3637,23 +3636,23 @@
       </c>
       <c r="AB23">
         <f t="shared" si="11"/>
-        <v>0.46400000000000002</v>
+        <v>0.44</v>
       </c>
       <c r="AC23">
         <f t="shared" si="12"/>
-        <v>0.46232960000000001</v>
+        <v>0.43841599999999997</v>
       </c>
       <c r="AD23">
         <f t="shared" si="13"/>
-        <v>0.73606612335026123</v>
+        <v>0.73092731826749635</v>
       </c>
       <c r="AE23">
         <f t="shared" si="14"/>
-        <v>1.4979809922451215</v>
+        <v>1.4867608135409596</v>
       </c>
       <c r="AF23">
         <f t="shared" si="15"/>
-        <v>1.3870194372640012</v>
+        <v>1.3766303829082958</v>
       </c>
       <c r="AG23">
         <f t="shared" si="16"/>
@@ -3752,23 +3751,23 @@
       </c>
       <c r="AB24">
         <f t="shared" si="11"/>
-        <v>0.46400000000000002</v>
+        <v>0.44</v>
       </c>
       <c r="AC24">
         <f t="shared" si="12"/>
-        <v>0.46232960000000001</v>
+        <v>0.43841599999999997</v>
       </c>
       <c r="AD24">
         <f t="shared" si="13"/>
-        <v>0.76191486889486026</v>
+        <v>0.75583349527346322</v>
       </c>
       <c r="AE24">
         <f t="shared" si="14"/>
-        <v>1.4964865920761574</v>
+        <v>1.4845092232630601</v>
       </c>
       <c r="AF24">
         <f t="shared" si="15"/>
-        <v>1.3856357334038494</v>
+        <v>1.374545577095426</v>
       </c>
       <c r="AG24">
         <f t="shared" si="16"/>
@@ -3867,23 +3866,23 @@
       </c>
       <c r="AB25">
         <f t="shared" si="11"/>
-        <v>0.46400000000000002</v>
+        <v>0.44</v>
       </c>
       <c r="AC25">
         <f t="shared" si="12"/>
-        <v>0.46232960000000001</v>
+        <v>0.43841599999999997</v>
       </c>
       <c r="AD25">
         <f t="shared" si="13"/>
-        <v>0.73457172318129715</v>
+        <v>0.72867572798959679</v>
       </c>
       <c r="AE25">
         <f t="shared" si="14"/>
-        <v>1.5315587316023676</v>
+        <v>1.5189147665042733</v>
       </c>
       <c r="AF25">
         <f t="shared" si="15"/>
-        <v>1.3674631532163994</v>
+        <v>1.3561738986645295</v>
       </c>
       <c r="AG25">
         <f t="shared" si="16"/>
@@ -3982,23 +3981,23 @@
       </c>
       <c r="AB26">
         <f t="shared" si="11"/>
-        <v>0.46400000000000002</v>
+        <v>0.44</v>
       </c>
       <c r="AC26">
         <f t="shared" si="12"/>
-        <v>0.46232960000000001</v>
+        <v>0.43841599999999997</v>
       </c>
       <c r="AD26">
         <f t="shared" si="13"/>
-        <v>0.79698700842107029</v>
+        <v>0.79023903851467647</v>
       </c>
       <c r="AE26">
         <f t="shared" si="14"/>
-        <v>1.5501392914421457</v>
+        <v>1.5384107772724693</v>
       </c>
       <c r="AF26">
         <f t="shared" si="15"/>
-        <v>1.3363269753811602</v>
+        <v>1.3262161873038529</v>
       </c>
       <c r="AG26">
         <f t="shared" si="16"/>
@@ -4097,23 +4096,23 @@
       </c>
       <c r="AB27">
         <f t="shared" si="11"/>
-        <v>0.46400000000000002</v>
+        <v>0.44</v>
       </c>
       <c r="AC27">
         <f t="shared" si="12"/>
-        <v>0.46232960000000001</v>
+        <v>0.43841599999999997</v>
       </c>
       <c r="AD27">
         <f t="shared" si="13"/>
-        <v>0.75315228302107551</v>
+        <v>0.74817173875779286</v>
       </c>
       <c r="AE27">
         <f t="shared" si="14"/>
-        <v>1.425243680584765</v>
+        <v>1.4151728489710891</v>
       </c>
       <c r="AF27">
         <f t="shared" si="15"/>
-        <v>1.2725390005221116</v>
+        <v>1.2635471865813295</v>
       </c>
       <c r="AG27">
         <f t="shared" si="16"/>
@@ -4212,23 +4211,23 @@
       </c>
       <c r="AB28">
         <f t="shared" si="11"/>
-        <v>0.46400000000000002</v>
+        <v>0.44</v>
       </c>
       <c r="AC28">
         <f t="shared" si="12"/>
-        <v>0.46232960000000001</v>
+        <v>0.43841599999999997</v>
       </c>
       <c r="AD28">
         <f t="shared" si="13"/>
-        <v>0.67209139756368952</v>
+        <v>0.66700111021329611</v>
       </c>
       <c r="AE28">
         <f t="shared" si="14"/>
-        <v>1.4278516682624731</v>
+        <v>1.416927645448419</v>
       </c>
       <c r="AF28">
         <f t="shared" si="15"/>
-        <v>1.2525014633881344</v>
+        <v>1.2429189872354554</v>
       </c>
       <c r="AG28">
         <f t="shared" si="16"/>
@@ -4327,23 +4326,23 @@
       </c>
       <c r="AB29">
         <f t="shared" si="11"/>
-        <v>0.46400000000000002</v>
+        <v>0.44</v>
       </c>
       <c r="AC29">
         <f t="shared" si="12"/>
-        <v>0.46232960000000001</v>
+        <v>0.43841599999999997</v>
       </c>
       <c r="AD29">
         <f t="shared" si="13"/>
-        <v>0.7557602706987836</v>
+        <v>0.74992653523512276</v>
       </c>
       <c r="AE29">
         <f t="shared" si="14"/>
-        <v>1.462840702926667</v>
+        <v>1.4519710896334477</v>
       </c>
       <c r="AF29">
         <f t="shared" si="15"/>
-        <v>1.2396955109548027</v>
+        <v>1.2304839742656337</v>
       </c>
       <c r="AG29">
         <f t="shared" si="16"/>
@@ -4442,23 +4441,23 @@
       </c>
       <c r="AB30">
         <f t="shared" si="11"/>
-        <v>0.46400000000000002</v>
+        <v>0.44</v>
       </c>
       <c r="AC30">
         <f t="shared" si="12"/>
-        <v>0.46232960000000001</v>
+        <v>0.43841599999999997</v>
       </c>
       <c r="AD30">
         <f t="shared" si="13"/>
-        <v>0.70708043222788342</v>
+        <v>0.70204455439832492</v>
       </c>
       <c r="AE30">
         <f t="shared" si="14"/>
-        <v>1.4076610408389105</v>
+        <v>1.3980253215770291</v>
       </c>
       <c r="AF30">
         <f t="shared" si="15"/>
-        <v>1.2568402150347415</v>
+        <v>1.2482368942652045</v>
       </c>
       <c r="AG30">
         <f t="shared" si="16"/>
@@ -4557,23 +4556,23 @@
       </c>
       <c r="AB31">
         <f t="shared" si="11"/>
-        <v>0.46400000000000002</v>
+        <v>0.44</v>
       </c>
       <c r="AC31">
         <f t="shared" si="12"/>
-        <v>0.46232960000000001</v>
+        <v>0.43841599999999997</v>
       </c>
       <c r="AD31">
         <f t="shared" si="13"/>
-        <v>0.70058060861102711</v>
+        <v>0.69598076717870416</v>
       </c>
       <c r="AE31">
         <f t="shared" si="14"/>
-        <v>1.4266553291804214</v>
+        <v>1.4160259043734955</v>
       </c>
       <c r="AF31">
         <f t="shared" si="15"/>
-        <v>1.3209771566485382</v>
+        <v>1.3111350966421254</v>
       </c>
       <c r="AG31">
         <f t="shared" si="16"/>
@@ -4672,23 +4671,23 @@
       </c>
       <c r="AB32">
         <f t="shared" si="11"/>
-        <v>0.46400000000000002</v>
+        <v>0.44</v>
       </c>
       <c r="AC32">
         <f t="shared" si="12"/>
-        <v>0.46232960000000001</v>
+        <v>0.43841599999999997</v>
       </c>
       <c r="AD32">
         <f t="shared" si="13"/>
-        <v>0.72607472056939426</v>
+        <v>0.72004513719479135</v>
       </c>
       <c r="AE32">
         <f t="shared" si="14"/>
-        <v>1.523725922709402</v>
+        <v>1.5119440550633048</v>
       </c>
       <c r="AF32">
         <f t="shared" si="15"/>
-        <v>1.3852053842812744</v>
+        <v>1.3744945955120951</v>
       </c>
       <c r="AG32">
         <f t="shared" si="16"/>
@@ -4787,23 +4786,23 @@
       </c>
       <c r="AB33">
         <f t="shared" si="11"/>
-        <v>0.46400000000000002</v>
+        <v>0.44</v>
       </c>
       <c r="AC33">
         <f t="shared" si="12"/>
-        <v>0.46232960000000001</v>
+        <v>0.43841599999999997</v>
       </c>
       <c r="AD33">
         <f t="shared" si="13"/>
-        <v>0.79765120214000784</v>
+        <v>0.7918989178685133</v>
       </c>
       <c r="AE33">
         <f t="shared" si="14"/>
-        <v>1.5266115057841048</v>
+        <v>1.5148491241645541</v>
       </c>
       <c r="AF33">
         <f t="shared" si="15"/>
-        <v>1.3878286416219132</v>
+        <v>1.3771355674223218</v>
       </c>
       <c r="AG33">
         <f t="shared" si="16"/>
@@ -4902,23 +4901,23 @@
       </c>
       <c r="AB34">
         <f t="shared" si="11"/>
-        <v>0.46400000000000002</v>
+        <v>0.44</v>
       </c>
       <c r="AC34">
         <f t="shared" si="12"/>
-        <v>0.46232960000000001</v>
+        <v>0.43841599999999997</v>
       </c>
       <c r="AD34">
         <f t="shared" si="13"/>
-        <v>0.72896030364409703</v>
+        <v>0.72295020629604079</v>
       </c>
       <c r="AE34">
         <f t="shared" si="14"/>
-        <v>1.5204438693194375</v>
+        <v>1.5088306531413087</v>
       </c>
       <c r="AF34">
         <f t="shared" si="15"/>
-        <v>1.3575391690352119</v>
+        <v>1.3471702260190255</v>
       </c>
       <c r="AG34">
         <f t="shared" si="16"/>
@@ -5017,23 +5016,23 @@
       </c>
       <c r="AB35">
         <f t="shared" si="11"/>
-        <v>0.46400000000000002</v>
+        <v>0.44</v>
       </c>
       <c r="AC35">
         <f t="shared" si="12"/>
-        <v>0.46232960000000001</v>
+        <v>0.43841599999999997</v>
       </c>
       <c r="AD35">
         <f t="shared" si="13"/>
-        <v>0.79148356567534051</v>
+        <v>0.78588044684526803</v>
       </c>
       <c r="AE35">
         <f t="shared" si="14"/>
-        <v>1.5005517401311921</v>
+        <v>1.4889849990462538</v>
       </c>
       <c r="AF35">
         <f t="shared" si="15"/>
-        <v>1.3162734562554317</v>
+        <v>1.3061271921458368</v>
       </c>
       <c r="AG35">
         <f t="shared" si="16"/>
@@ -5132,23 +5131,23 @@
       </c>
       <c r="AB36">
         <f t="shared" si="11"/>
-        <v>0.46400000000000002</v>
+        <v>0.44</v>
       </c>
       <c r="AC36">
         <f t="shared" si="12"/>
-        <v>0.46232960000000001</v>
+        <v>0.43841599999999997</v>
       </c>
       <c r="AD36">
         <f t="shared" si="13"/>
-        <v>0.70906817445585157</v>
+        <v>0.70310455220098578</v>
       </c>
       <c r="AE36">
         <f t="shared" si="14"/>
-        <v>1.4298869297409327</v>
+        <v>1.4183262111942501</v>
       </c>
       <c r="AF36">
         <f t="shared" si="15"/>
-        <v>1.2766847586972612</v>
+        <v>1.2663626885662946</v>
       </c>
       <c r="AG36">
         <f t="shared" si="16"/>
@@ -5247,23 +5246,23 @@
       </c>
       <c r="AB37">
         <f t="shared" si="11"/>
-        <v>0.46400000000000002</v>
+        <v>0.44</v>
       </c>
       <c r="AC37">
         <f t="shared" si="12"/>
-        <v>0.46232960000000001</v>
+        <v>0.43841599999999997</v>
       </c>
       <c r="AD37">
         <f t="shared" si="13"/>
-        <v>0.7208187552850811</v>
+        <v>0.71522165899326418</v>
       </c>
       <c r="AE37">
         <f t="shared" si="14"/>
-        <v>1.5473091601889728</v>
+        <v>1.5345260629304556</v>
       </c>
       <c r="AF37">
         <f t="shared" si="15"/>
-        <v>1.3112789493126888</v>
+        <v>1.300445816042759</v>
       </c>
       <c r="AG37">
         <f t="shared" si="16"/>
@@ -5362,23 +5361,23 @@
       </c>
       <c r="AB38">
         <f t="shared" si="11"/>
-        <v>0.46400000000000002</v>
+        <v>0.44</v>
       </c>
       <c r="AC38">
         <f t="shared" si="12"/>
-        <v>0.46232960000000001</v>
+        <v>0.43841599999999997</v>
       </c>
       <c r="AD38">
         <f t="shared" si="13"/>
-        <v>0.8264904049038917</v>
+        <v>0.81930440393719128</v>
       </c>
       <c r="AE38">
         <f t="shared" si="14"/>
-        <v>1.4128701562468591</v>
+        <v>1.3997298891463963</v>
       </c>
       <c r="AF38">
         <f t="shared" si="15"/>
-        <v>1.4417042410682235</v>
+        <v>1.4282958052514247</v>
       </c>
       <c r="AG38">
         <f t="shared" si="16"/>
@@ -5477,23 +5476,23 @@
       </c>
       <c r="AB39">
         <f t="shared" si="11"/>
-        <v>0.46400000000000002</v>
+        <v>0.44</v>
       </c>
       <c r="AC39">
         <f t="shared" si="12"/>
-        <v>0.46232960000000001</v>
+        <v>0.43841599999999997</v>
       </c>
       <c r="AD39">
         <f t="shared" si="13"/>
-        <v>0.58637975134296738</v>
+        <v>0.58042548520920501</v>
       </c>
       <c r="AE39">
         <f t="shared" si="14"/>
-        <v>1.0563747827997414</v>
+        <v>1.046747767677024</v>
       </c>
       <c r="AF39">
         <f t="shared" si="15"/>
-        <v>0.91066791620667364</v>
+        <v>0.90236876523881393</v>
       </c>
       <c r="AG39">
         <f t="shared" si="16"/>
@@ -5592,23 +5591,23 @@
       </c>
       <c r="AB40">
         <f t="shared" si="11"/>
-        <v>0.46400000000000002</v>
+        <v>0.44</v>
       </c>
       <c r="AC40">
         <f t="shared" si="12"/>
-        <v>0.46232960000000001</v>
+        <v>0.43841599999999997</v>
       </c>
       <c r="AD40">
         <f t="shared" si="13"/>
-        <v>0.4699950314567739</v>
+        <v>0.46632228246781915</v>
       </c>
       <c r="AE40">
         <f t="shared" si="14"/>
-        <v>1.1222581424172193</v>
+        <v>1.1152666134049478</v>
       </c>
       <c r="AF40">
         <f t="shared" si="15"/>
-        <v>0.69275193976371563</v>
+        <v>0.68843618111416527</v>
       </c>
       <c r="AG40">
         <f t="shared" si="16"/>
@@ -5707,23 +5706,23 @@
       </c>
       <c r="AB41">
         <f t="shared" si="11"/>
-        <v>0.46400000000000002</v>
+        <v>0.44</v>
       </c>
       <c r="AC41">
         <f t="shared" si="12"/>
-        <v>0.46232960000000001</v>
+        <v>0.43841599999999997</v>
       </c>
       <c r="AD41">
         <f t="shared" si="13"/>
-        <v>0.65226311096044554</v>
+        <v>0.64894433093712878</v>
       </c>
       <c r="AE41">
         <f t="shared" si="14"/>
-        <v>1.4352684499401023</v>
+        <v>1.4249866235194841</v>
       </c>
       <c r="AF41">
         <f t="shared" si="15"/>
-        <v>0.98306058215075498</v>
+        <v>0.9760182352873179</v>
       </c>
       <c r="AG41">
         <f t="shared" si="16"/>
@@ -5822,23 +5821,23 @@
       </c>
       <c r="AB42">
         <f t="shared" si="11"/>
-        <v>0.46400000000000002</v>
+        <v>0.44</v>
       </c>
       <c r="AC42">
         <f t="shared" si="12"/>
-        <v>0.46232960000000001</v>
+        <v>0.43841599999999997</v>
       </c>
       <c r="AD42">
         <f t="shared" si="13"/>
-        <v>0.78300533897965674</v>
+        <v>0.77604229258235546</v>
       </c>
       <c r="AE42">
         <f t="shared" si="14"/>
-        <v>1.4475828905156558</v>
+        <v>1.4365874390987097</v>
       </c>
       <c r="AF42">
         <f t="shared" si="15"/>
-        <v>1.1674055568674644</v>
+        <v>1.158538257337669</v>
       </c>
       <c r="AG42">
         <f t="shared" si="16"/>
@@ -5937,23 +5936,23 @@
       </c>
       <c r="AB43">
         <f t="shared" si="11"/>
-        <v>0.46400000000000002</v>
+        <v>0.44</v>
       </c>
       <c r="AC43">
         <f t="shared" si="12"/>
-        <v>0.46232960000000001</v>
+        <v>0.43841599999999997</v>
       </c>
       <c r="AD43">
         <f t="shared" si="13"/>
-        <v>0.66457755153599907</v>
+        <v>0.66054514651635432</v>
       </c>
       <c r="AE43">
         <f t="shared" si="14"/>
-        <v>1.3645278294262675</v>
+        <v>1.3555629528514914</v>
       </c>
       <c r="AF43">
         <f t="shared" si="15"/>
-        <v>1.1969542363388312</v>
+        <v>1.1890903095188523</v>
       </c>
       <c r="AG43">
         <f t="shared" si="16"/>
@@ -6052,23 +6051,23 @@
       </c>
       <c r="AB44">
         <f t="shared" si="11"/>
-        <v>0.46400000000000002</v>
+        <v>0.44</v>
       </c>
       <c r="AC44">
         <f t="shared" si="12"/>
-        <v>0.46232960000000001</v>
+        <v>0.43841599999999997</v>
       </c>
       <c r="AD44">
         <f t="shared" si="13"/>
-        <v>0.69995027789026831</v>
+        <v>0.69501780633513699</v>
       </c>
       <c r="AE44">
         <f t="shared" si="14"/>
-        <v>1.4973486579143751</v>
+        <v>1.485952798344</v>
       </c>
       <c r="AF44">
         <f t="shared" si="15"/>
-        <v>1.3369184445664062</v>
+        <v>1.3267435699499999</v>
       </c>
       <c r="AG44">
         <f t="shared" si="16"/>
@@ -6167,23 +6166,23 @@
       </c>
       <c r="AB45">
         <f t="shared" si="11"/>
-        <v>0.46400000000000002</v>
+        <v>0.44</v>
       </c>
       <c r="AC45">
         <f t="shared" si="12"/>
-        <v>0.46232960000000001</v>
+        <v>0.43841599999999997</v>
       </c>
       <c r="AD45">
         <f t="shared" si="13"/>
-        <v>0.7973983800241069</v>
+        <v>0.79093499200886286</v>
       </c>
       <c r="AE45">
         <f t="shared" si="14"/>
-        <v>1.5042529649077836</v>
+        <v>1.4926168647156861</v>
       </c>
       <c r="AF45">
         <f t="shared" si="15"/>
-        <v>1.3430830043819495</v>
+        <v>1.3326936292104339</v>
       </c>
       <c r="AG45">
         <f t="shared" si="16"/>
@@ -6282,23 +6281,23 @@
       </c>
       <c r="AB46">
         <f t="shared" si="11"/>
-        <v>0.46400000000000002</v>
+        <v>0.44</v>
       </c>
       <c r="AC46">
         <f t="shared" si="12"/>
-        <v>0.46232960000000001</v>
+        <v>0.43841599999999997</v>
       </c>
       <c r="AD46">
         <f t="shared" si="13"/>
-        <v>0.7068545848836767</v>
+        <v>0.70168187270682314</v>
       </c>
       <c r="AE46">
         <f t="shared" si="14"/>
-        <v>1.4176432470483182</v>
+        <v>1.4065626676239007</v>
       </c>
       <c r="AF46">
         <f t="shared" si="15"/>
-        <v>1.2887665882257437</v>
+        <v>1.278693334203546</v>
       </c>
       <c r="AG46">
         <f t="shared" si="16"/>
@@ -6397,23 +6396,23 @@
       </c>
       <c r="AB47">
         <f t="shared" si="11"/>
-        <v>0.46400000000000002</v>
+        <v>0.44</v>
       </c>
       <c r="AC47">
         <f t="shared" si="12"/>
-        <v>0.46232960000000001</v>
+        <v>0.43841599999999997</v>
       </c>
       <c r="AD47">
         <f t="shared" si="13"/>
-        <v>0.71078866216464143</v>
+        <v>0.70488079491707756</v>
       </c>
       <c r="AE47">
         <f t="shared" si="14"/>
-        <v>1.5113094258161932</v>
+        <v>1.4994852464442991</v>
       </c>
       <c r="AF47">
         <f t="shared" si="15"/>
-        <v>1.3493834159073153</v>
+        <v>1.3388261128966956</v>
       </c>
       <c r="AG47">
         <f t="shared" si="16"/>
@@ -6512,23 +6511,23 @@
       </c>
       <c r="AB48">
         <f t="shared" si="11"/>
-        <v>0.46400000000000002</v>
+        <v>0.44</v>
       </c>
       <c r="AC48">
         <f t="shared" si="12"/>
-        <v>0.46232960000000001</v>
+        <v>0.43841599999999997</v>
       </c>
       <c r="AD48">
         <f t="shared" si="13"/>
-        <v>0.80052076365155189</v>
+        <v>0.79460445152722148</v>
       </c>
       <c r="AE48">
         <f t="shared" si="14"/>
-        <v>1.5615063802749689</v>
+        <v>1.5494314514838101</v>
       </c>
       <c r="AF48">
         <f t="shared" si="15"/>
-        <v>1.3697424388376922</v>
+        <v>1.3591503960384301</v>
       </c>
       <c r="AG48">
         <f t="shared" si="16"/>
@@ -6627,23 +6626,23 @@
       </c>
       <c r="AB49">
         <f t="shared" si="11"/>
-        <v>0.46400000000000002</v>
+        <v>0.44</v>
       </c>
       <c r="AC49">
         <f t="shared" si="12"/>
-        <v>0.46232960000000001</v>
+        <v>0.43841599999999997</v>
       </c>
       <c r="AD49">
         <f t="shared" si="13"/>
-        <v>0.76098561662341702</v>
+        <v>0.75482699995658875</v>
       </c>
       <c r="AE49">
         <f t="shared" si="14"/>
-        <v>1.4735330491769523</v>
+        <v>1.4629231082446013</v>
       </c>
       <c r="AF49">
         <f t="shared" si="15"/>
-        <v>1.3156545081937072</v>
+        <v>1.3061813466469654</v>
       </c>
       <c r="AG49">
         <f t="shared" si="16"/>
@@ -6742,23 +6741,23 @@
       </c>
       <c r="AB50">
         <f t="shared" si="11"/>
-        <v>0.46400000000000002</v>
+        <v>0.44</v>
       </c>
       <c r="AC50">
         <f t="shared" si="12"/>
-        <v>0.46232960000000001</v>
+        <v>0.43841599999999997</v>
       </c>
       <c r="AD50">
         <f t="shared" si="13"/>
-        <v>0.71254743255353525</v>
+        <v>0.70809610828801239</v>
       </c>
       <c r="AE50">
         <f t="shared" si="14"/>
-        <v>1.4358683487928672</v>
+        <v>1.4260103805422437</v>
       </c>
       <c r="AF50">
         <f t="shared" si="15"/>
-        <v>1.3295077303637659</v>
+        <v>1.3203799819835589</v>
       </c>
       <c r="AG50">
         <f t="shared" si="16"/>
@@ -6854,24 +6853,24 @@
         <v>0.39999999999999997</v>
       </c>
       <c r="AB51">
-        <f t="shared" si="11"/>
-        <v>0.46400000000000002</v>
+        <f>1.1 * AA51</f>
+        <v>0.44</v>
       </c>
       <c r="AC51">
         <f t="shared" si="12"/>
-        <v>0.46232960000000001</v>
-      </c>
-      <c r="AD51" s="4">
+        <v>0.43841599999999997</v>
+      </c>
+      <c r="AD51">
         <f t="shared" si="13"/>
-        <v>0.72332091623933192</v>
+        <v>0.71791427225423132</v>
       </c>
       <c r="AE51" s="1">
         <f t="shared" si="14"/>
-        <v>0.72332091623933192</v>
+        <v>0.71791427225423132</v>
       </c>
       <c r="AF51" s="1">
         <f t="shared" si="15"/>
-        <v>-2.5559042976654837E-2</v>
+        <v>-2.5367995486015239E-2</v>
       </c>
       <c r="AG51">
         <f t="shared" si="16"/>
@@ -6957,11 +6956,11 @@
       </c>
       <c r="AE52" s="1">
         <f t="shared" si="14"/>
-        <v>0.51130710006439306</v>
+        <v>0.50455350742054139</v>
       </c>
       <c r="AF52" s="1">
         <f t="shared" si="15"/>
-        <v>-1.7729095009167584E-2</v>
+        <v>-1.7494920506953584E-2</v>
       </c>
       <c r="AG52" s="1">
         <f t="shared" si="16"/>
@@ -7059,24 +7058,24 @@
         <v>0.39999999999999997</v>
       </c>
       <c r="AB53">
-        <f t="shared" si="11"/>
-        <v>0.46400000000000002</v>
+        <f>1.1 * AA53</f>
+        <v>0.44</v>
       </c>
       <c r="AC53">
         <f t="shared" si="12"/>
-        <v>0.46232960000000001</v>
+        <v>0.43841599999999997</v>
       </c>
       <c r="AD53">
         <f t="shared" si="13"/>
-        <v>0.51130710006439306</v>
+        <v>0.50455350742054139</v>
       </c>
       <c r="AE53">
         <f t="shared" si="14"/>
-        <v>1.0114642365905597</v>
+        <v>1.0019631913421958</v>
       </c>
       <c r="AF53">
         <f t="shared" si="15"/>
-        <v>0.79020643483637476</v>
+        <v>0.78278374323609046</v>
       </c>
       <c r="AG53">
         <f t="shared" si="16"/>
@@ -7174,24 +7173,24 @@
         <v>0.39999999999999997</v>
       </c>
       <c r="AB54">
-        <f t="shared" si="11"/>
-        <v>0.46400000000000002</v>
+        <f t="shared" ref="AB54:AB81" si="19">1.1 * AA54</f>
+        <v>0.44</v>
       </c>
       <c r="AC54">
         <f t="shared" si="12"/>
-        <v>0.46232960000000001</v>
+        <v>0.43841599999999997</v>
       </c>
       <c r="AD54">
         <f t="shared" si="13"/>
-        <v>0.50015713652616656</v>
+        <v>0.49740968392165452</v>
       </c>
       <c r="AE54">
         <f t="shared" si="14"/>
-        <v>1.2042946932357927</v>
+        <v>1.1964762609541384</v>
       </c>
       <c r="AF54">
         <f t="shared" si="15"/>
-        <v>0.98712679773425638</v>
+        <v>0.98071824668371999</v>
       </c>
       <c r="AG54">
         <f t="shared" si="16"/>
@@ -7289,24 +7288,24 @@
         <v>0.39999999999999997</v>
       </c>
       <c r="AB55">
-        <f t="shared" si="11"/>
-        <v>0.46400000000000002</v>
+        <f t="shared" si="19"/>
+        <v>0.44</v>
       </c>
       <c r="AC55">
         <f t="shared" si="12"/>
-        <v>0.46232960000000001</v>
+        <v>0.43841599999999997</v>
       </c>
       <c r="AD55">
         <f t="shared" si="13"/>
-        <v>0.70413755670962619</v>
+        <v>0.69906657703248387</v>
       </c>
       <c r="AE55">
         <f t="shared" si="14"/>
-        <v>1.4496239318778685</v>
+        <v>1.4390313587731729</v>
       </c>
       <c r="AF55">
         <f t="shared" si="15"/>
-        <v>1.2715999402437443</v>
+        <v>1.2623082094501519</v>
       </c>
       <c r="AG55">
         <f t="shared" si="16"/>
@@ -7404,24 +7403,24 @@
         <v>0.39999999999999997</v>
       </c>
       <c r="AB56">
-        <f t="shared" si="11"/>
-        <v>0.46400000000000002</v>
+        <f t="shared" si="19"/>
+        <v>0.44</v>
       </c>
       <c r="AC56">
         <f t="shared" si="12"/>
-        <v>0.46232960000000001</v>
+        <v>0.43841599999999997</v>
       </c>
       <c r="AD56">
         <f t="shared" si="13"/>
-        <v>0.74548637516824223</v>
+        <v>0.73996478174068903</v>
       </c>
       <c r="AE56">
         <f t="shared" si="14"/>
-        <v>1.5647966652124428</v>
+        <v>1.5520780939281402</v>
       </c>
       <c r="AF56">
         <f t="shared" si="15"/>
-        <v>1.3971398796539667</v>
+        <v>1.3857840124358394</v>
       </c>
       <c r="AG56">
         <f t="shared" si="16"/>
@@ -7519,24 +7518,24 @@
         <v>0.39999999999999997</v>
       </c>
       <c r="AB57">
-        <f t="shared" si="11"/>
-        <v>0.46400000000000002</v>
+        <f t="shared" si="19"/>
+        <v>0.44</v>
       </c>
       <c r="AC57">
         <f t="shared" si="12"/>
-        <v>0.46232960000000001</v>
+        <v>0.43841599999999997</v>
       </c>
       <c r="AD57">
         <f t="shared" si="13"/>
-        <v>0.81931029004420064</v>
+        <v>0.81211331218745109</v>
       </c>
       <c r="AE57">
         <f t="shared" si="14"/>
-        <v>1.5671800623704646</v>
+        <v>1.5540100038694682</v>
       </c>
       <c r="AF57">
         <f t="shared" si="15"/>
-        <v>1.3992679128307719</v>
+        <v>1.3875089320263108</v>
       </c>
       <c r="AG57">
         <f t="shared" si="16"/>
@@ -7634,24 +7633,24 @@
         <v>0.39999999999999997</v>
       </c>
       <c r="AB58">
-        <f t="shared" si="11"/>
-        <v>0.46400000000000002</v>
+        <f t="shared" si="19"/>
+        <v>0.44</v>
       </c>
       <c r="AC58">
         <f t="shared" si="12"/>
-        <v>0.46232960000000001</v>
+        <v>0.43841599999999997</v>
       </c>
       <c r="AD58">
         <f t="shared" si="13"/>
-        <v>0.74786977232626395</v>
+        <v>0.74189669168201711</v>
       </c>
       <c r="AE58">
         <f t="shared" si="14"/>
-        <v>1.5607637486969121</v>
+        <v>1.5471395504221594</v>
       </c>
       <c r="AF58">
         <f t="shared" si="15"/>
-        <v>1.3935390613365286</v>
+        <v>1.3813745985912136</v>
       </c>
       <c r="AG58">
         <f t="shared" si="16"/>
@@ -7749,24 +7748,24 @@
         <v>0.39999999999999997</v>
       </c>
       <c r="AB59">
-        <f t="shared" si="11"/>
-        <v>0.46400000000000002</v>
+        <f t="shared" si="19"/>
+        <v>0.44</v>
       </c>
       <c r="AC59">
         <f t="shared" si="12"/>
-        <v>0.46232960000000001</v>
+        <v>0.43841599999999997</v>
       </c>
       <c r="AD59">
         <f t="shared" si="13"/>
-        <v>0.81289397637064809</v>
+        <v>0.80524285874014234</v>
       </c>
       <c r="AE59">
         <f t="shared" si="14"/>
-        <v>1.6034756453257606</v>
+        <v>1.5892823366072426</v>
       </c>
       <c r="AF59">
         <f t="shared" si="15"/>
-        <v>1.4316746833265719</v>
+        <v>1.4190020862564665</v>
       </c>
       <c r="AG59">
         <f t="shared" si="16"/>
@@ -7864,24 +7863,24 @@
         <v>0.39999999999999997</v>
       </c>
       <c r="AB60">
-        <f t="shared" si="11"/>
-        <v>0.46400000000000002</v>
+        <f t="shared" si="19"/>
+        <v>0.44</v>
       </c>
       <c r="AC60">
         <f t="shared" si="12"/>
-        <v>0.46232960000000001</v>
+        <v>0.43841599999999997</v>
       </c>
       <c r="AD60">
         <f t="shared" si="13"/>
-        <v>0.7905816689551125</v>
+        <v>0.78403947786710027</v>
       </c>
       <c r="AE60">
         <f t="shared" si="14"/>
-        <v>1.625586896080204</v>
+        <v>1.6116976778313583</v>
       </c>
       <c r="AF60">
         <f t="shared" si="15"/>
-        <v>1.4259534176142141</v>
+        <v>1.413769892834525</v>
       </c>
       <c r="AG60">
         <f t="shared" si="16"/>
@@ -7979,24 +7978,24 @@
         <v>0.39999999999999997</v>
       </c>
       <c r="AB61">
-        <f t="shared" si="11"/>
-        <v>0.46400000000000002</v>
+        <f t="shared" si="19"/>
+        <v>0.44</v>
       </c>
       <c r="AC61">
         <f t="shared" si="12"/>
-        <v>0.46232960000000001</v>
+        <v>0.43841599999999997</v>
       </c>
       <c r="AD61">
         <f t="shared" si="13"/>
-        <v>0.83500522712509162</v>
+        <v>0.82765819996425805</v>
       </c>
       <c r="AE61">
         <f t="shared" si="14"/>
-        <v>1.5643166667997881</v>
+        <v>1.5526731920666932</v>
       </c>
       <c r="AF61">
         <f t="shared" si="15"/>
-        <v>1.3485488506894725</v>
+        <v>1.3385113724712874</v>
       </c>
       <c r="AG61">
         <f t="shared" si="16"/>
@@ -8094,24 +8093,24 @@
         <v>0.39999999999999997</v>
       </c>
       <c r="AB62">
-        <f t="shared" si="11"/>
-        <v>0.46400000000000002</v>
+        <f t="shared" si="19"/>
+        <v>0.44</v>
       </c>
       <c r="AC62">
         <f t="shared" si="12"/>
-        <v>0.46232960000000001</v>
+        <v>0.43841599999999997</v>
       </c>
       <c r="AD62">
         <f t="shared" si="13"/>
-        <v>0.72931143967469647</v>
+        <v>0.72501499210243503</v>
       </c>
       <c r="AE62">
         <f t="shared" si="14"/>
-        <v>1.4369738053675354</v>
+        <v>1.4269099449418907</v>
       </c>
       <c r="AF62">
         <f t="shared" si="15"/>
-        <v>1.3063398230613956</v>
+        <v>1.2971908590380823</v>
       </c>
       <c r="AG62">
         <f t="shared" si="16"/>
@@ -8209,24 +8208,24 @@
         <v>0.39999999999999997</v>
       </c>
       <c r="AB63">
-        <f t="shared" si="11"/>
-        <v>0.46400000000000002</v>
+        <f t="shared" si="19"/>
+        <v>0.44</v>
       </c>
       <c r="AC63">
         <f t="shared" si="12"/>
-        <v>0.46232960000000001</v>
+        <v>0.43841599999999997</v>
       </c>
       <c r="AD63">
         <f t="shared" si="13"/>
-        <v>0.7076623656928388</v>
+        <v>0.7018949528394558</v>
       </c>
       <c r="AE63">
         <f t="shared" si="14"/>
-        <v>1.4434950450862918</v>
+        <v>1.4317541567468774</v>
       </c>
       <c r="AF63">
         <f t="shared" si="15"/>
-        <v>1.3365694861910109</v>
+        <v>1.3256982932841457</v>
       </c>
       <c r="AG63">
         <f t="shared" si="16"/>
@@ -8324,24 +8323,24 @@
         <v>0.39999999999999997</v>
       </c>
       <c r="AB64">
-        <f t="shared" si="11"/>
-        <v>0.46400000000000002</v>
+        <f t="shared" si="19"/>
+        <v>0.44</v>
       </c>
       <c r="AC64">
         <f t="shared" si="12"/>
-        <v>0.46232960000000001</v>
+        <v>0.43841599999999997</v>
       </c>
       <c r="AD64">
         <f t="shared" si="13"/>
-        <v>0.73583267939345298</v>
+        <v>0.72985920390742176</v>
       </c>
       <c r="AE64">
         <f t="shared" si="14"/>
-        <v>1.5571701663830839</v>
+        <v>1.5439864574578426</v>
       </c>
       <c r="AF64">
         <f t="shared" si="15"/>
-        <v>1.3659387424413019</v>
+        <v>1.3543740854893358</v>
       </c>
       <c r="AG64">
         <f t="shared" si="16"/>
@@ -8439,24 +8438,24 @@
         <v>0.39999999999999997</v>
       </c>
       <c r="AB65">
-        <f t="shared" si="11"/>
-        <v>0.46400000000000002</v>
+        <f t="shared" si="19"/>
+        <v>0.44</v>
       </c>
       <c r="AC65">
         <f t="shared" si="12"/>
-        <v>0.46232960000000001</v>
+        <v>0.43841599999999997</v>
       </c>
       <c r="AD65">
         <f t="shared" si="13"/>
-        <v>0.82133748698963083</v>
+        <v>0.8141272535504207</v>
       </c>
       <c r="AE65">
         <f t="shared" si="14"/>
-        <v>1.5251913554202494</v>
+        <v>1.5126955479613096</v>
       </c>
       <c r="AF65">
         <f t="shared" si="15"/>
-        <v>1.337887153877412</v>
+        <v>1.3269259192643068</v>
       </c>
       <c r="AG65">
         <f t="shared" si="16"/>
@@ -8554,24 +8553,24 @@
         <v>0.39999999999999997</v>
       </c>
       <c r="AB66">
-        <f t="shared" si="11"/>
-        <v>0.46400000000000002</v>
+        <f t="shared" si="19"/>
+        <v>0.44</v>
       </c>
       <c r="AC66">
         <f t="shared" si="12"/>
-        <v>0.46232960000000001</v>
+        <v>0.43841599999999997</v>
       </c>
       <c r="AD66">
         <f t="shared" si="13"/>
-        <v>0.70385386843061859</v>
+        <v>0.69856829441088886</v>
       </c>
       <c r="AE66">
         <f t="shared" si="14"/>
-        <v>1.5221565701667723</v>
+        <v>1.5100349340516246</v>
       </c>
       <c r="AF66">
         <f t="shared" si="15"/>
-        <v>1.3590683662203322</v>
+        <v>1.3482454768318075</v>
       </c>
       <c r="AG66">
         <f t="shared" si="16"/>
@@ -8625,35 +8624,35 @@
         <v>0.99639999999999995</v>
       </c>
       <c r="Q67">
-        <f t="shared" ref="Q67:Q81" si="19">($H67-$E67)/50</f>
+        <f t="shared" ref="Q67:Q81" si="20">($H67-$E67)/50</f>
         <v>0.57999999999999996</v>
       </c>
       <c r="R67">
-        <f t="shared" ref="R67:R80" si="20">(I67 - E67) / 50</f>
+        <f t="shared" ref="R67:R80" si="21">(I67 - E67) / 50</f>
         <v>1.1200000000000001</v>
       </c>
       <c r="S67">
-        <f t="shared" ref="S67:S82" si="21">(G67-E67)/50</f>
+        <f t="shared" ref="S67:S82" si="22">(G67-E67)/50</f>
         <v>0.74</v>
       </c>
       <c r="T67">
-        <f t="shared" ref="T67:T80" si="22">(I67-G67)/50</f>
+        <f t="shared" ref="T67:T80" si="23">(I67-G67)/50</f>
         <v>0.38</v>
       </c>
       <c r="U67">
-        <f t="shared" ref="U67:U82" si="23">(F67-E67)/50</f>
+        <f t="shared" ref="U67:U82" si="24">(F67-E67)/50</f>
         <v>0.16</v>
       </c>
       <c r="V67">
-        <f t="shared" ref="V67:V81" si="24">(G67-H67)/50</f>
+        <f t="shared" ref="V67:V81" si="25">(G67-H67)/50</f>
         <v>0.16</v>
       </c>
       <c r="W67">
-        <f t="shared" ref="W67:W81" si="25">U67+V67</f>
+        <f t="shared" ref="W67:W81" si="26">U67+V67</f>
         <v>0.32</v>
       </c>
       <c r="X67">
-        <f t="shared" ref="X67:X81" si="26">(H67-F67)/50</f>
+        <f t="shared" ref="X67:X81" si="27">(H67-F67)/50</f>
         <v>0.42</v>
       </c>
       <c r="Y67" s="2">
@@ -8665,28 +8664,28 @@
         <v>0.4</v>
       </c>
       <c r="AA67">
-        <f t="shared" ref="AA67:AA81" si="27">Y67/Z67</f>
+        <f t="shared" ref="AA67:AA81" si="28">Y67/Z67</f>
         <v>0.39999999999999997</v>
       </c>
       <c r="AB67">
-        <f t="shared" ref="AB67:AB81" si="28">1.12 * AA67 * AA67 + 0.547 * AA67 + 0.066</f>
-        <v>0.46400000000000002</v>
+        <f t="shared" si="19"/>
+        <v>0.44</v>
       </c>
       <c r="AC67">
         <f t="shared" ref="AC67:AC81" si="29">AB67*P67</f>
-        <v>0.46232960000000001</v>
+        <v>0.43841599999999997</v>
       </c>
       <c r="AD67">
         <f t="shared" ref="AD67:AD81" si="30">2 * SQRT(2 * P67 * N67 - N67 * N67) + 2 * SQRT(2 * AC67 * O67 - O67 * O67)</f>
-        <v>0.8183027017361536</v>
+        <v>0.81146663964073573</v>
       </c>
       <c r="AE67">
         <f t="shared" ref="AE67:AE80" si="31">AD67+AD68</f>
-        <v>1.5241242600683211</v>
+        <v>1.5118191282594173</v>
       </c>
       <c r="AF67">
         <f t="shared" ref="AF67:AF80" si="32">AE67/R67</f>
-        <v>1.3608252322038581</v>
+        <v>1.3498385073744796</v>
       </c>
       <c r="AG67">
         <f t="shared" ref="AG67:AG81" si="33">60/Q67</f>
@@ -8740,35 +8739,35 @@
         <v>0.99639999999999995</v>
       </c>
       <c r="Q68">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>0.54</v>
       </c>
       <c r="R68">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>1.1399999999999999</v>
       </c>
       <c r="S68">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>0.7</v>
       </c>
       <c r="T68">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>0.44</v>
       </c>
       <c r="U68">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v>0.16</v>
       </c>
       <c r="V68">
-        <f t="shared" si="24"/>
+        <f t="shared" si="25"/>
         <v>0.16</v>
       </c>
       <c r="W68">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v>0.32</v>
       </c>
       <c r="X68">
-        <f t="shared" si="26"/>
+        <f t="shared" si="27"/>
         <v>0.38</v>
       </c>
       <c r="Y68" s="2">
@@ -8780,28 +8779,28 @@
         <v>0.4</v>
       </c>
       <c r="AA68">
-        <f t="shared" si="27"/>
+        <f t="shared" si="28"/>
         <v>0.39999999999999997</v>
       </c>
       <c r="AB68">
-        <f t="shared" si="28"/>
-        <v>0.46400000000000002</v>
+        <f t="shared" si="19"/>
+        <v>0.44</v>
       </c>
       <c r="AC68">
         <f t="shared" si="29"/>
-        <v>0.46232960000000001</v>
+        <v>0.43841599999999997</v>
       </c>
       <c r="AD68">
         <f t="shared" si="30"/>
-        <v>0.70582155833216753</v>
+        <v>0.70035248861868149</v>
       </c>
       <c r="AE68">
         <f t="shared" si="31"/>
-        <v>1.5470579205777406</v>
+        <v>1.5348784023949444</v>
       </c>
       <c r="AF68">
         <f t="shared" si="32"/>
-        <v>1.3570683513839832</v>
+        <v>1.3463845635043374</v>
       </c>
       <c r="AG68">
         <f t="shared" si="33"/>
@@ -8855,35 +8854,35 @@
         <v>0.99639999999999995</v>
       </c>
       <c r="Q69">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>0.6</v>
       </c>
       <c r="R69">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>1.1599999999999999</v>
       </c>
       <c r="S69">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>0.76</v>
       </c>
       <c r="T69">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>0.4</v>
       </c>
       <c r="U69">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v>0.16</v>
       </c>
       <c r="V69">
-        <f t="shared" si="24"/>
+        <f t="shared" si="25"/>
         <v>0.16</v>
       </c>
       <c r="W69">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v>0.32</v>
       </c>
       <c r="X69">
-        <f t="shared" si="26"/>
+        <f t="shared" si="27"/>
         <v>0.44</v>
       </c>
       <c r="Y69" s="2">
@@ -8895,28 +8894,28 @@
         <v>0.4</v>
       </c>
       <c r="AA69">
-        <f t="shared" si="27"/>
+        <f t="shared" si="28"/>
         <v>0.39999999999999997</v>
       </c>
       <c r="AB69">
-        <f t="shared" si="28"/>
-        <v>0.46400000000000002</v>
+        <f t="shared" si="19"/>
+        <v>0.44</v>
       </c>
       <c r="AC69">
         <f t="shared" si="29"/>
-        <v>0.46232960000000001</v>
+        <v>0.43841599999999997</v>
       </c>
       <c r="AD69">
         <f t="shared" si="30"/>
-        <v>0.84123636224557308</v>
+        <v>0.83452591377626284</v>
       </c>
       <c r="AE69">
         <f t="shared" si="31"/>
-        <v>1.5584982398698468</v>
+        <v>1.5467057227589025</v>
       </c>
       <c r="AF69">
         <f t="shared" si="32"/>
-        <v>1.3435329654050405</v>
+        <v>1.3333670023783644</v>
       </c>
       <c r="AG69">
         <f t="shared" si="33"/>
@@ -8970,35 +8969,35 @@
         <v>0.99639999999999995</v>
       </c>
       <c r="Q70">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>0.56000000000000005</v>
       </c>
       <c r="R70">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>1.1200000000000001</v>
       </c>
       <c r="S70">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>0.7</v>
       </c>
       <c r="T70">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>0.42</v>
       </c>
       <c r="U70">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v>0.16</v>
       </c>
       <c r="V70">
-        <f t="shared" si="24"/>
+        <f t="shared" si="25"/>
         <v>0.14000000000000001</v>
       </c>
       <c r="W70">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v>0.30000000000000004</v>
       </c>
       <c r="X70">
-        <f t="shared" si="26"/>
+        <f t="shared" si="27"/>
         <v>0.4</v>
       </c>
       <c r="Y70" s="2">
@@ -9010,28 +9009,28 @@
         <v>0.4</v>
       </c>
       <c r="AA70">
-        <f t="shared" si="27"/>
+        <f t="shared" si="28"/>
         <v>0.39999999999999997</v>
       </c>
       <c r="AB70">
-        <f t="shared" si="28"/>
-        <v>0.46400000000000002</v>
+        <f t="shared" si="19"/>
+        <v>0.44</v>
       </c>
       <c r="AC70">
         <f t="shared" si="29"/>
-        <v>0.46232960000000001</v>
+        <v>0.43841599999999997</v>
       </c>
       <c r="AD70">
         <f t="shared" si="30"/>
-        <v>0.71726187762427374</v>
+        <v>0.71217980898263966</v>
       </c>
       <c r="AE70">
         <f t="shared" si="31"/>
-        <v>1.4301878335616411</v>
+        <v>1.4196718152453724</v>
       </c>
       <c r="AF70">
         <f t="shared" si="32"/>
-        <v>1.2769534228228938</v>
+        <v>1.2675641207547967</v>
       </c>
       <c r="AG70">
         <f t="shared" si="33"/>
@@ -9085,35 +9084,35 @@
         <v>0.99639999999999995</v>
       </c>
       <c r="Q71">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>0.56000000000000005</v>
       </c>
       <c r="R71">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>1.1200000000000001</v>
       </c>
       <c r="S71">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>0.72</v>
       </c>
       <c r="T71">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>0.4</v>
       </c>
       <c r="U71">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v>0.14000000000000001</v>
       </c>
       <c r="V71">
-        <f t="shared" si="24"/>
+        <f t="shared" si="25"/>
         <v>0.16</v>
       </c>
       <c r="W71">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v>0.30000000000000004</v>
       </c>
       <c r="X71">
-        <f t="shared" si="26"/>
+        <f t="shared" si="27"/>
         <v>0.42</v>
       </c>
       <c r="Y71" s="2">
@@ -9125,28 +9124,28 @@
         <v>0.4</v>
       </c>
       <c r="AA71">
-        <f t="shared" si="27"/>
+        <f t="shared" si="28"/>
         <v>0.39999999999999997</v>
       </c>
       <c r="AB71">
-        <f t="shared" si="28"/>
-        <v>0.46400000000000002</v>
+        <f t="shared" si="19"/>
+        <v>0.44</v>
       </c>
       <c r="AC71">
         <f t="shared" si="29"/>
-        <v>0.46232960000000001</v>
+        <v>0.43841599999999997</v>
       </c>
       <c r="AD71">
         <f t="shared" si="30"/>
-        <v>0.71292595593736752</v>
+        <v>0.70749200626273279</v>
       </c>
       <c r="AE71">
         <f t="shared" si="31"/>
-        <v>1.4409313407048607</v>
+        <v>1.4304395166389632</v>
       </c>
       <c r="AF71">
         <f t="shared" si="32"/>
-        <v>1.286545839915054</v>
+        <v>1.277178139856217</v>
       </c>
       <c r="AG71">
         <f t="shared" si="33"/>
@@ -9200,35 +9199,35 @@
         <v>0.99639999999999995</v>
       </c>
       <c r="Q72">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>0.56000000000000005</v>
       </c>
       <c r="R72">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>1.1200000000000001</v>
       </c>
       <c r="S72">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>0.72</v>
       </c>
       <c r="T72">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>0.4</v>
       </c>
       <c r="U72">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v>0.16</v>
       </c>
       <c r="V72">
-        <f t="shared" si="24"/>
+        <f t="shared" si="25"/>
         <v>0.16</v>
       </c>
       <c r="W72">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v>0.32</v>
       </c>
       <c r="X72">
-        <f t="shared" si="26"/>
+        <f t="shared" si="27"/>
         <v>0.4</v>
       </c>
       <c r="Y72" s="2">
@@ -9240,28 +9239,28 @@
         <v>0.4</v>
       </c>
       <c r="AA72">
-        <f t="shared" si="27"/>
+        <f t="shared" si="28"/>
         <v>0.39999999999999997</v>
       </c>
       <c r="AB72">
-        <f t="shared" si="28"/>
-        <v>0.46400000000000002</v>
+        <f t="shared" si="19"/>
+        <v>0.44</v>
       </c>
       <c r="AC72">
         <f t="shared" si="29"/>
-        <v>0.46232960000000001</v>
+        <v>0.43841599999999997</v>
       </c>
       <c r="AD72">
         <f t="shared" si="30"/>
-        <v>0.72800538476749332</v>
+        <v>0.7229475103762304</v>
       </c>
       <c r="AE72">
         <f t="shared" si="31"/>
-        <v>1.4889325065283359</v>
+        <v>1.4776414764089609</v>
       </c>
       <c r="AF72">
         <f t="shared" si="32"/>
-        <v>1.3294040236860141</v>
+        <v>1.319322746793715</v>
       </c>
       <c r="AG72">
         <f t="shared" si="33"/>
@@ -9315,35 +9314,35 @@
         <v>0.99639999999999995</v>
       </c>
       <c r="Q73">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>0.56000000000000005</v>
       </c>
       <c r="R73">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>1.1200000000000001</v>
       </c>
       <c r="S73">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>0.72</v>
       </c>
       <c r="T73">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>0.4</v>
       </c>
       <c r="U73">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v>0.16</v>
       </c>
       <c r="V73">
-        <f t="shared" si="24"/>
+        <f t="shared" si="25"/>
         <v>0.16</v>
       </c>
       <c r="W73">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v>0.32</v>
       </c>
       <c r="X73">
-        <f t="shared" si="26"/>
+        <f t="shared" si="27"/>
         <v>0.4</v>
       </c>
       <c r="Y73" s="2">
@@ -9355,28 +9354,28 @@
         <v>0.4</v>
       </c>
       <c r="AA73">
-        <f t="shared" si="27"/>
+        <f t="shared" si="28"/>
         <v>0.39999999999999997</v>
       </c>
       <c r="AB73">
-        <f t="shared" si="28"/>
-        <v>0.46400000000000002</v>
+        <f t="shared" si="19"/>
+        <v>0.44</v>
       </c>
       <c r="AC73">
         <f t="shared" si="29"/>
-        <v>0.46232960000000001</v>
+        <v>0.43841599999999997</v>
       </c>
       <c r="AD73">
         <f t="shared" si="30"/>
-        <v>0.76092712176084265</v>
+        <v>0.75469396603273065</v>
       </c>
       <c r="AE73">
         <f t="shared" si="31"/>
-        <v>1.4722351455132261</v>
+        <v>1.4598690343868554</v>
       </c>
       <c r="AF73">
         <f t="shared" si="32"/>
-        <v>1.314495665636809</v>
+        <v>1.3034544949882636</v>
       </c>
       <c r="AG73">
         <f t="shared" si="33"/>
@@ -9430,35 +9429,35 @@
         <v>0.99639999999999995</v>
       </c>
       <c r="Q74">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>0.56000000000000005</v>
       </c>
       <c r="R74">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>1.18</v>
       </c>
       <c r="S74">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>0.74</v>
       </c>
       <c r="T74">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>0.44</v>
       </c>
       <c r="U74">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v>0.16</v>
       </c>
       <c r="V74">
-        <f t="shared" si="24"/>
+        <f t="shared" si="25"/>
         <v>0.18</v>
       </c>
       <c r="W74">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v>0.33999999999999997</v>
       </c>
       <c r="X74">
-        <f t="shared" si="26"/>
+        <f t="shared" si="27"/>
         <v>0.4</v>
       </c>
       <c r="Y74" s="2">
@@ -9470,28 +9469,28 @@
         <v>0.4</v>
       </c>
       <c r="AA74">
-        <f t="shared" si="27"/>
+        <f t="shared" si="28"/>
         <v>0.39999999999999997</v>
       </c>
       <c r="AB74">
-        <f t="shared" si="28"/>
-        <v>0.46400000000000002</v>
+        <f t="shared" si="19"/>
+        <v>0.44</v>
       </c>
       <c r="AC74">
         <f t="shared" si="29"/>
-        <v>0.46232960000000001</v>
+        <v>0.43841599999999997</v>
       </c>
       <c r="AD74">
         <f t="shared" si="30"/>
-        <v>0.71130802375238344</v>
+        <v>0.70517506835412491</v>
       </c>
       <c r="AE74">
         <f t="shared" si="31"/>
-        <v>1.5344657978816059</v>
+        <v>1.5213402433534111</v>
       </c>
       <c r="AF74">
         <f t="shared" si="32"/>
-        <v>1.3003947439674626</v>
+        <v>1.2892713926723824</v>
       </c>
       <c r="AG74">
         <f t="shared" si="33"/>
@@ -9545,35 +9544,35 @@
         <v>0.99639999999999995</v>
       </c>
       <c r="Q75">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>0.62</v>
       </c>
       <c r="R75">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>1.18</v>
       </c>
       <c r="S75">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>0.78</v>
       </c>
       <c r="T75">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>0.4</v>
       </c>
       <c r="U75">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v>0.18</v>
       </c>
       <c r="V75">
-        <f t="shared" si="24"/>
+        <f t="shared" si="25"/>
         <v>0.16</v>
       </c>
       <c r="W75">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v>0.33999999999999997</v>
       </c>
       <c r="X75">
-        <f t="shared" si="26"/>
+        <f t="shared" si="27"/>
         <v>0.44</v>
       </c>
       <c r="Y75" s="2">
@@ -9585,28 +9584,28 @@
         <v>0.4</v>
       </c>
       <c r="AA75">
-        <f t="shared" si="27"/>
+        <f t="shared" si="28"/>
         <v>0.39999999999999997</v>
       </c>
       <c r="AB75">
-        <f t="shared" si="28"/>
-        <v>0.46400000000000002</v>
+        <f t="shared" si="19"/>
+        <v>0.44</v>
       </c>
       <c r="AC75">
         <f t="shared" si="29"/>
-        <v>0.46232960000000001</v>
+        <v>0.43841599999999997</v>
       </c>
       <c r="AD75">
         <f t="shared" si="30"/>
-        <v>0.82315777412922242</v>
+        <v>0.81616517499928631</v>
       </c>
       <c r="AE75">
         <f t="shared" si="31"/>
-        <v>1.547713903789798</v>
+        <v>1.5348783293280759</v>
       </c>
       <c r="AF75">
         <f t="shared" si="32"/>
-        <v>1.3116219523642356</v>
+        <v>1.3007443468882001</v>
       </c>
       <c r="AG75">
         <f t="shared" si="33"/>
@@ -9660,35 +9659,35 @@
         <v>0.99639999999999995</v>
       </c>
       <c r="Q76">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>0.56000000000000005</v>
       </c>
       <c r="R76">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>1.1200000000000001</v>
       </c>
       <c r="S76">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>0.72</v>
       </c>
       <c r="T76">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>0.4</v>
       </c>
       <c r="U76">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v>0.16</v>
       </c>
       <c r="V76">
-        <f t="shared" si="24"/>
+        <f t="shared" si="25"/>
         <v>0.16</v>
       </c>
       <c r="W76">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v>0.32</v>
       </c>
       <c r="X76">
-        <f t="shared" si="26"/>
+        <f t="shared" si="27"/>
         <v>0.4</v>
       </c>
       <c r="Y76" s="2">
@@ -9700,28 +9699,28 @@
         <v>0.4</v>
       </c>
       <c r="AA76">
-        <f t="shared" si="27"/>
+        <f t="shared" si="28"/>
         <v>0.39999999999999997</v>
       </c>
       <c r="AB76">
-        <f t="shared" si="28"/>
-        <v>0.46400000000000002</v>
+        <f t="shared" si="19"/>
+        <v>0.44</v>
       </c>
       <c r="AC76">
         <f t="shared" si="29"/>
-        <v>0.46232960000000001</v>
+        <v>0.43841599999999997</v>
       </c>
       <c r="AD76">
         <f t="shared" si="30"/>
-        <v>0.72455612966057548</v>
+        <v>0.71871315432878946</v>
       </c>
       <c r="AE76">
         <f t="shared" si="31"/>
-        <v>1.467826888089901</v>
+        <v>1.4557929572591659</v>
       </c>
       <c r="AF76">
         <f t="shared" si="32"/>
-        <v>1.31055972150884</v>
+        <v>1.2998151404099694</v>
       </c>
       <c r="AG76">
         <f t="shared" si="33"/>
@@ -9775,35 +9774,35 @@
         <v>0.99639999999999995</v>
       </c>
       <c r="Q77">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>0.56000000000000005</v>
       </c>
       <c r="R77">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>1.1599999999999999</v>
       </c>
       <c r="S77">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>0.74</v>
       </c>
       <c r="T77">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>0.42</v>
       </c>
       <c r="U77">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v>0.16</v>
       </c>
       <c r="V77">
-        <f t="shared" si="24"/>
+        <f t="shared" si="25"/>
         <v>0.18</v>
       </c>
       <c r="W77">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v>0.33999999999999997</v>
       </c>
       <c r="X77">
-        <f t="shared" si="26"/>
+        <f t="shared" si="27"/>
         <v>0.4</v>
       </c>
       <c r="Y77" s="2">
@@ -9815,28 +9814,28 @@
         <v>0.4</v>
       </c>
       <c r="AA77">
-        <f t="shared" si="27"/>
+        <f t="shared" si="28"/>
         <v>0.39999999999999997</v>
       </c>
       <c r="AB77">
-        <f t="shared" si="28"/>
-        <v>0.46400000000000002</v>
+        <f t="shared" si="19"/>
+        <v>0.44</v>
       </c>
       <c r="AC77">
         <f t="shared" si="29"/>
-        <v>0.46232960000000001</v>
+        <v>0.43841599999999997</v>
       </c>
       <c r="AD77">
         <f t="shared" si="30"/>
-        <v>0.74327075842932555</v>
+        <v>0.73707980293037634</v>
       </c>
       <c r="AE77">
         <f t="shared" si="31"/>
-        <v>1.5489751217294718</v>
+        <v>1.5367868237251483</v>
       </c>
       <c r="AF77">
         <f t="shared" si="32"/>
-        <v>1.335323380801269</v>
+        <v>1.3248162273492659</v>
       </c>
       <c r="AG77">
         <f t="shared" si="33"/>
@@ -9890,35 +9889,35 @@
         <v>0.99639999999999995</v>
       </c>
       <c r="Q78">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>0.6</v>
       </c>
       <c r="R78">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>1.1599999999999999</v>
       </c>
       <c r="S78">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>0.74</v>
       </c>
       <c r="T78">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>0.42</v>
       </c>
       <c r="U78">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v>0.18</v>
       </c>
       <c r="V78">
-        <f t="shared" si="24"/>
+        <f t="shared" si="25"/>
         <v>0.14000000000000001</v>
       </c>
       <c r="W78">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v>0.32</v>
       </c>
       <c r="X78">
-        <f t="shared" si="26"/>
+        <f t="shared" si="27"/>
         <v>0.42</v>
       </c>
       <c r="Y78" s="2">
@@ -9930,28 +9929,28 @@
         <v>0.4</v>
       </c>
       <c r="AA78">
-        <f t="shared" si="27"/>
+        <f t="shared" si="28"/>
         <v>0.39999999999999997</v>
       </c>
       <c r="AB78">
-        <f t="shared" si="28"/>
-        <v>0.46400000000000002</v>
+        <f t="shared" si="19"/>
+        <v>0.44</v>
       </c>
       <c r="AC78">
         <f t="shared" si="29"/>
-        <v>0.46232960000000001</v>
+        <v>0.43841599999999997</v>
       </c>
       <c r="AD78">
         <f t="shared" si="30"/>
-        <v>0.80570436330014616</v>
+        <v>0.79970702079477207</v>
       </c>
       <c r="AE78">
         <f t="shared" si="31"/>
-        <v>1.5002241197510173</v>
+        <v>1.4890899819665018</v>
       </c>
       <c r="AF78">
         <f t="shared" si="32"/>
-        <v>1.2932966549577736</v>
+        <v>1.2836982603159499</v>
       </c>
       <c r="AG78">
         <f t="shared" si="33"/>
@@ -10005,35 +10004,35 @@
         <v>0.99639999999999995</v>
       </c>
       <c r="Q79">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>0.56000000000000005</v>
       </c>
       <c r="R79">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>1.1200000000000001</v>
       </c>
       <c r="S79">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>0.72</v>
       </c>
       <c r="T79">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>0.4</v>
       </c>
       <c r="U79">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v>0.14000000000000001</v>
       </c>
       <c r="V79">
-        <f t="shared" si="24"/>
+        <f t="shared" si="25"/>
         <v>0.16</v>
       </c>
       <c r="W79">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v>0.30000000000000004</v>
       </c>
       <c r="X79">
-        <f t="shared" si="26"/>
+        <f t="shared" si="27"/>
         <v>0.42</v>
       </c>
       <c r="Y79" s="2">
@@ -10045,28 +10044,28 @@
         <v>0.4</v>
       </c>
       <c r="AA79">
-        <f t="shared" si="27"/>
+        <f t="shared" si="28"/>
         <v>0.39999999999999997</v>
       </c>
       <c r="AB79">
-        <f t="shared" si="28"/>
-        <v>0.46400000000000002</v>
+        <f t="shared" si="19"/>
+        <v>0.44</v>
       </c>
       <c r="AC79">
         <f t="shared" si="29"/>
-        <v>0.46232960000000001</v>
+        <v>0.43841599999999997</v>
       </c>
       <c r="AD79">
         <f t="shared" si="30"/>
-        <v>0.69451975645087105</v>
+        <v>0.68938296117172959</v>
       </c>
       <c r="AE79">
         <f t="shared" si="31"/>
-        <v>1.4228448981325794</v>
+        <v>1.412437442102068</v>
       </c>
       <c r="AF79">
         <f t="shared" si="32"/>
-        <v>1.2703972304755171</v>
+        <v>1.2611048590197034</v>
       </c>
       <c r="AG79">
         <f t="shared" si="33"/>
@@ -10120,35 +10119,35 @@
         <v>0.99639999999999995</v>
       </c>
       <c r="Q80">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>0.56000000000000005</v>
       </c>
       <c r="R80">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>1.1200000000000001</v>
       </c>
       <c r="S80">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>0.7</v>
       </c>
       <c r="T80">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>0.42</v>
       </c>
       <c r="U80">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v>0.16</v>
       </c>
       <c r="V80">
-        <f t="shared" si="24"/>
+        <f t="shared" si="25"/>
         <v>0.14000000000000001</v>
       </c>
       <c r="W80">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v>0.30000000000000004</v>
       </c>
       <c r="X80">
-        <f t="shared" si="26"/>
+        <f t="shared" si="27"/>
         <v>0.4</v>
       </c>
       <c r="Y80" s="2">
@@ -10160,28 +10159,28 @@
         <v>0.4</v>
       </c>
       <c r="AA80">
-        <f t="shared" si="27"/>
+        <f t="shared" si="28"/>
         <v>0.39999999999999997</v>
       </c>
       <c r="AB80">
-        <f t="shared" si="28"/>
-        <v>0.46400000000000002</v>
+        <f t="shared" si="19"/>
+        <v>0.44</v>
       </c>
       <c r="AC80">
         <f t="shared" si="29"/>
-        <v>0.46232960000000001</v>
+        <v>0.43841599999999997</v>
       </c>
       <c r="AD80">
         <f t="shared" si="30"/>
-        <v>0.72832514168170848</v>
+        <v>0.72305448093033853</v>
       </c>
       <c r="AE80">
         <f t="shared" si="31"/>
-        <v>1.5296452380580852</v>
+        <v>1.5175238329758616</v>
       </c>
       <c r="AF80">
         <f t="shared" si="32"/>
-        <v>1.3657546768375759</v>
+        <v>1.3549319937284476</v>
       </c>
       <c r="AG80">
         <f t="shared" si="33"/>
@@ -10233,29 +10232,29 @@
         <v>0.99639999999999995</v>
       </c>
       <c r="Q81">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>0.56000000000000005</v>
       </c>
       <c r="R81" s="1"/>
       <c r="S81">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>0.74</v>
       </c>
       <c r="T81" s="1"/>
       <c r="U81">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v>0.14000000000000001</v>
       </c>
       <c r="V81">
-        <f t="shared" si="24"/>
+        <f t="shared" si="25"/>
         <v>0.18</v>
       </c>
       <c r="W81">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v>0.32</v>
       </c>
       <c r="X81">
-        <f t="shared" si="26"/>
+        <f t="shared" si="27"/>
         <v>0.42</v>
       </c>
       <c r="Y81" s="2">
@@ -10267,20 +10266,20 @@
         <v>0.4</v>
       </c>
       <c r="AA81">
-        <f t="shared" si="27"/>
+        <f t="shared" si="28"/>
         <v>0.39999999999999997</v>
       </c>
       <c r="AB81">
-        <f t="shared" si="28"/>
-        <v>0.46400000000000002</v>
+        <f t="shared" si="19"/>
+        <v>0.44</v>
       </c>
       <c r="AC81">
         <f t="shared" si="29"/>
-        <v>0.46232960000000001</v>
+        <v>0.43841599999999997</v>
       </c>
       <c r="AD81">
         <f t="shared" si="30"/>
-        <v>0.80132009637637669</v>
+        <v>0.79446935204552305</v>
       </c>
       <c r="AE81" s="1"/>
       <c r="AF81" s="1"/>
@@ -10325,12 +10324,12 @@
       <c r="Q82" s="1"/>
       <c r="R82" s="1"/>
       <c r="S82">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>0.76</v>
       </c>
       <c r="T82" s="1"/>
       <c r="U82">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v>0.18</v>
       </c>
       <c r="V82" s="1"/>

</xml_diff>